<commit_message>
Added phase 2 and phase 3
</commit_message>
<xml_diff>
--- a/ImageFiles.xlsx
+++ b/ImageFiles.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_F25DC773A252ABEACE02ECCA639E5F2C5ADE58A0" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2F299B8B-3AF1-44E9-9B8A-5D94BB2676D3}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="11_F25DC773A252ABEACE02ECCA639E5F2C5ADE58A0" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{FC6049FE-6CCE-4525-A918-6265F3BD6DA2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="4215" windowWidth="21360" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,19 +31,19 @@
     <t>ImageFile</t>
   </si>
   <si>
-    <t>images/Face1.jpg</t>
-  </si>
-  <si>
-    <t>images/Face2.jpg</t>
-  </si>
-  <si>
-    <t>images/Face3.jpg</t>
-  </si>
-  <si>
     <t>Shock</t>
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>images/Face1.BMP</t>
+  </si>
+  <si>
+    <t>images/Face2.BMP</t>
+  </si>
+  <si>
+    <t>images/Face3.BMP</t>
   </si>
 </sst>
 </file>
@@ -373,12 +373,14 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -386,15 +388,15 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -405,7 +407,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -416,7 +418,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>2</v>

</xml_diff>